<commit_message>
upated employee data xlsx with the valid reporter
</commit_message>
<xml_diff>
--- a/data/employeeData.xlsx
+++ b/data/employeeData.xlsx
@@ -109,9 +109,6 @@
     <t>Bangalore</t>
   </si>
   <si>
-    <t>chandana.vennam@optimworks.com</t>
-  </si>
-  <si>
     <t>Spanda</t>
   </si>
   <si>
@@ -263,6 +260,9 @@
   </si>
   <si>
     <t>rahul@gmail.com</t>
+  </si>
+  <si>
+    <t>mounikareddy@optimworks.com</t>
   </si>
 </sst>
 </file>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,7 +671,7 @@
     <col min="12" max="12" width="11.88671875" customWidth="1"/>
     <col min="13" max="13" width="14.33203125" customWidth="1"/>
     <col min="14" max="14" width="19" customWidth="1"/>
-    <col min="17" max="17" width="21" customWidth="1"/>
+    <col min="17" max="17" width="44.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -735,10 +735,10 @@
         <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -776,22 +776,22 @@
       <c r="P2" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" t="s">
-        <v>31</v>
+      <c r="Q2" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
         <v>19</v>
@@ -829,22 +829,22 @@
       <c r="P3" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" t="s">
-        <v>31</v>
+      <c r="Q3" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -853,51 +853,51 @@
         <v>20</v>
       </c>
       <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
         <v>35</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>36</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>37</v>
-      </c>
-      <c r="J4" t="s">
-        <v>38</v>
       </c>
       <c r="K4" t="s">
         <v>25</v>
       </c>
       <c r="L4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" t="s">
         <v>39</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>40</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>41</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>42</v>
       </c>
-      <c r="P4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>31</v>
+      <c r="Q4" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
@@ -906,51 +906,51 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
         <v>46</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>47</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>48</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>49</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>50</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>51</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>52</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>53</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>54</v>
       </c>
-      <c r="P5" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>31</v>
+      <c r="Q5" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
-        <v>57</v>
-      </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -959,90 +959,90 @@
         <v>20</v>
       </c>
       <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
         <v>58</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>59</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>60</v>
-      </c>
-      <c r="J6" t="s">
-        <v>61</v>
       </c>
       <c r="K6" t="s">
         <v>25</v>
       </c>
       <c r="L6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" t="s">
         <v>62</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
+        <v>59</v>
+      </c>
+      <c r="O6" t="s">
         <v>63</v>
       </c>
-      <c r="N6" t="s">
-        <v>60</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>64</v>
       </c>
-      <c r="P6" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>31</v>
+      <c r="Q6" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
         <v>66</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G7" s="2">
         <v>37931</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" t="s">
         <v>60</v>
-      </c>
-      <c r="J7" t="s">
-        <v>61</v>
       </c>
       <c r="K7" t="s">
         <v>25</v>
       </c>
       <c r="L7" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" t="s">
         <v>62</v>
       </c>
-      <c r="M7" t="s">
-        <v>63</v>
-      </c>
       <c r="N7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P7" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>31</v>
+        <v>64</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1053,6 +1053,8 @@
     <hyperlink ref="D4" r:id="rId4"/>
     <hyperlink ref="D5" r:id="rId5"/>
     <hyperlink ref="D6" r:id="rId6"/>
+    <hyperlink ref="Q2" r:id="rId7"/>
+    <hyperlink ref="Q3:Q7" r:id="rId8" display="mounikareddy@optimworks.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>

</xml_diff>